<commit_message>
- Bestellisten bis auf Spulen/Ferrite zur Entkopplung vervollständigt - Oberer Widerstand im Spannungsteiler an 7,2V von 16k auf 14k Reduziert (7,5V -> 3,3V)
</commit_message>
<xml_diff>
--- a/kicad_ucboard/ucboard_Teileliste.xlsx
+++ b/kicad_ucboard/ucboard_Teileliste.xlsx
@@ -891,9 +891,6 @@
     <t>R22</t>
   </si>
   <si>
-    <t>16k</t>
-  </si>
-  <si>
     <t>P9</t>
   </si>
   <si>
@@ -1195,6 +1192,9 @@
   </si>
   <si>
     <t>R67</t>
+  </si>
+  <si>
+    <t>14k</t>
   </si>
 </sst>
 </file>
@@ -2038,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2081,250 +2081,628 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>1084340</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2">
+        <v>0.56499999999999995</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>1146032</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>4.25</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>373</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>374</v>
+      </c>
+      <c r="D4" t="s">
+        <v>378</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1202826</v>
+      </c>
+      <c r="G4" t="s">
+        <v>377</v>
+      </c>
+      <c r="H4" t="s">
+        <v>376</v>
+      </c>
+      <c r="I4">
+        <v>0.29699999999999999</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>1564957</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>1.33</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>1696320</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>4.4000000000000004</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>1696320</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>4.4000000000000004</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>296</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>1715855</v>
+      </c>
+      <c r="G8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I8">
+        <v>1.74</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>321</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>1772204</v>
+      </c>
+      <c r="G9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I9">
+        <v>56.5</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>1206</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>1828835</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10">
+        <v>0.154</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>1206</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>1828835</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11">
+        <v>0.154</v>
       </c>
       <c r="J11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>361</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12">
+        <v>1206</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12">
+        <v>1828835</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12">
+        <v>0.154</v>
       </c>
       <c r="J12" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>1206</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>1828835</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13">
+        <v>0.154</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>277</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14">
+        <v>1831089</v>
+      </c>
+      <c r="G14" t="s">
+        <v>280</v>
+      </c>
+      <c r="H14" t="s">
+        <v>278</v>
+      </c>
+      <c r="I14">
+        <v>0.224</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>349</v>
+        <v>285</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>277</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F15">
+        <v>1831089</v>
+      </c>
+      <c r="G15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H15" t="s">
+        <v>278</v>
+      </c>
+      <c r="I15">
+        <v>0.224</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>277</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16">
+        <v>1831089</v>
+      </c>
+      <c r="G16" t="s">
+        <v>280</v>
+      </c>
+      <c r="H16" t="s">
+        <v>278</v>
+      </c>
+      <c r="I16">
+        <v>0.224</v>
       </c>
       <c r="J16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>353</v>
+        <v>193</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>194</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>1842347</v>
+      </c>
+      <c r="G17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H17" t="s">
+        <v>196</v>
+      </c>
+      <c r="I17">
+        <v>0.58099999999999996</v>
       </c>
       <c r="J17" t="s">
-        <v>46</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>383</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>1857299</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>387</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>1857299</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>315</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>1857299</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>2061651</v>
+      </c>
+      <c r="G21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21">
+        <v>0.51200000000000001</v>
       </c>
       <c r="J21" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
+      <c r="D22">
+        <v>603</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>2346901</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22">
+        <v>8.5800000000000001E-2</v>
+      </c>
       <c r="J22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>603</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>2346901</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23">
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J23" t="s">
         <v>22</v>
@@ -2332,10 +2710,28 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>363</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>603</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>2346901</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24">
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
@@ -2343,10 +2739,28 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>364</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>603</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>2346901</v>
+      </c>
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25">
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
@@ -2354,654 +2768,897 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>243</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>244</v>
+      </c>
+      <c r="C26" t="s">
+        <v>247</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>2469429</v>
+      </c>
+      <c r="G26" t="s">
+        <v>246</v>
+      </c>
+      <c r="I26">
+        <v>0.66100000000000003</v>
       </c>
       <c r="J26" t="s">
-        <v>22</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>331</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>244</v>
+      </c>
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <v>2469429</v>
+      </c>
+      <c r="G27" t="s">
+        <v>246</v>
+      </c>
+      <c r="I27">
+        <v>0.66100000000000003</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>199</v>
+      </c>
+      <c r="D28">
+        <v>805</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <v>7568584</v>
+      </c>
+      <c r="G28" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28">
+        <v>0.22700000000000001</v>
       </c>
       <c r="J28" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>252</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>23</v>
+        <v>199</v>
+      </c>
+      <c r="D29">
+        <v>805</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <v>7568584</v>
+      </c>
+      <c r="G29" t="s">
+        <v>201</v>
+      </c>
+      <c r="I29">
+        <v>0.22700000000000001</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I30">
+        <v>9.58</v>
       </c>
       <c r="J30" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
+        <v>159</v>
+      </c>
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" t="s">
+        <v>161</v>
+      </c>
+      <c r="I31">
+        <v>7.39</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>355</v>
+      </c>
+      <c r="D32" t="s">
+        <v>360</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>358</v>
+      </c>
+      <c r="G32" t="s">
+        <v>359</v>
+      </c>
+      <c r="H32" t="s">
+        <v>357</v>
+      </c>
+      <c r="I32">
+        <v>0.24</v>
       </c>
       <c r="J32" t="s">
-        <v>22</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>70</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33">
+        <v>0.48</v>
       </c>
       <c r="J33" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>182</v>
+      </c>
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" t="s">
+        <v>185</v>
+      </c>
+      <c r="I34">
+        <v>0.63</v>
       </c>
       <c r="J34" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>249</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" t="s">
+        <v>132</v>
+      </c>
+      <c r="I35">
+        <v>0.22</v>
       </c>
       <c r="J35" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>251</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" t="s">
+        <v>132</v>
+      </c>
+      <c r="I36">
+        <v>0.22</v>
       </c>
       <c r="J36" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>259</v>
+      </c>
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" t="s">
+        <v>132</v>
+      </c>
+      <c r="I37">
+        <v>0.22</v>
       </c>
       <c r="J37" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>287</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>130</v>
+      </c>
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" t="s">
+        <v>133</v>
+      </c>
+      <c r="G38" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" t="s">
+        <v>132</v>
+      </c>
+      <c r="I38">
+        <v>0.22</v>
       </c>
       <c r="J38" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>320</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>124</v>
+      </c>
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39">
+        <v>0.26</v>
       </c>
       <c r="J39" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>270</v>
+        <v>204</v>
       </c>
       <c r="B40" t="s">
-        <v>271</v>
+        <v>205</v>
+      </c>
+      <c r="D40" t="s">
+        <v>210</v>
+      </c>
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" t="s">
+        <v>208</v>
+      </c>
+      <c r="G40" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" t="s">
+        <v>207</v>
+      </c>
+      <c r="I40">
+        <v>1.2</v>
       </c>
       <c r="J40" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="B41" t="s">
-        <v>271</v>
+        <v>213</v>
+      </c>
+      <c r="D41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>208</v>
+      </c>
+      <c r="G41" t="s">
+        <v>214</v>
+      </c>
+      <c r="H41" t="s">
+        <v>207</v>
+      </c>
+      <c r="I41">
+        <v>1.2</v>
       </c>
       <c r="J41" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>381</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>271</v>
+        <v>118</v>
+      </c>
+      <c r="D42" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" t="s">
+        <v>121</v>
+      </c>
+      <c r="I42">
+        <v>0.09</v>
       </c>
       <c r="J42" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>382</v>
+        <v>215</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>216</v>
+      </c>
+      <c r="D43" t="s">
+        <v>220</v>
+      </c>
+      <c r="E43" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" t="s">
+        <v>218</v>
+      </c>
+      <c r="G43" t="s">
+        <v>219</v>
+      </c>
+      <c r="I43">
+        <v>0.12</v>
       </c>
       <c r="J43" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>221</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>222</v>
+      </c>
+      <c r="D44" t="s">
+        <v>220</v>
+      </c>
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" t="s">
+        <v>218</v>
+      </c>
+      <c r="G44" t="s">
+        <v>219</v>
+      </c>
+      <c r="I44">
+        <v>0.12</v>
       </c>
       <c r="J44" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>106</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" t="s">
+        <v>109</v>
+      </c>
+      <c r="I45">
+        <v>0.12</v>
       </c>
       <c r="J45" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>337</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>338</v>
+      </c>
+      <c r="D46" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" t="s">
+        <v>340</v>
+      </c>
+      <c r="G46" t="s">
+        <v>341</v>
+      </c>
+      <c r="I46">
+        <v>0.16</v>
       </c>
       <c r="J46" t="s">
-        <v>46</v>
+        <v>339</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>102</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
       </c>
       <c r="J47" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>268</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>99</v>
+      </c>
+      <c r="D48" t="s">
+        <v>75</v>
       </c>
       <c r="J48" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>155</v>
+      </c>
+      <c r="D49" t="s">
+        <v>75</v>
       </c>
       <c r="J49" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>283</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>157</v>
+      </c>
+      <c r="D50" t="s">
+        <v>75</v>
       </c>
       <c r="J50" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>290</v>
+      </c>
+      <c r="D51" t="s">
+        <v>292</v>
       </c>
       <c r="J51" t="s">
-        <v>46</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>304</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>97</v>
       </c>
       <c r="J52" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>311</v>
+        <v>191</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>192</v>
+      </c>
+      <c r="D53" t="s">
+        <v>97</v>
       </c>
       <c r="J53" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>317</v>
+        <v>189</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>190</v>
+      </c>
+      <c r="D54" t="s">
+        <v>97</v>
       </c>
       <c r="J54" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>319</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>93</v>
       </c>
       <c r="J55" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>326</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>180</v>
+      </c>
+      <c r="D56" t="s">
+        <v>177</v>
       </c>
       <c r="J56" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>390</v>
+        <v>174</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>175</v>
+      </c>
+      <c r="D57" t="s">
+        <v>177</v>
       </c>
       <c r="J57" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" t="s">
-        <v>79</v>
+        <v>175</v>
+      </c>
+      <c r="D58" t="s">
+        <v>177</v>
       </c>
       <c r="J58" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>371</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>372</v>
+      </c>
+      <c r="D59" t="s">
+        <v>177</v>
       </c>
       <c r="J59" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>171</v>
+      </c>
+      <c r="D60" t="s">
+        <v>173</v>
       </c>
       <c r="J60" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>266</v>
+        <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>267</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1E-3</v>
+        <v>165</v>
+      </c>
+      <c r="D61" t="s">
+        <v>167</v>
       </c>
       <c r="J61" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>288</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>289</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1E-3</v>
+        <v>169</v>
+      </c>
+      <c r="D62" t="s">
+        <v>167</v>
       </c>
       <c r="J62" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>241</v>
+      </c>
+      <c r="D63" t="s">
+        <v>122</v>
       </c>
       <c r="J63" t="s">
-        <v>46</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>237</v>
+      </c>
+      <c r="D64" t="s">
+        <v>239</v>
       </c>
       <c r="J64" t="s">
-        <v>46</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="B65" t="s">
-        <v>244</v>
-      </c>
-      <c r="C65" t="s">
-        <v>247</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65">
-        <v>2469429</v>
-      </c>
-      <c r="G65" t="s">
-        <v>246</v>
-      </c>
-      <c r="I65">
-        <v>0.66100000000000003</v>
+        <v>188</v>
       </c>
       <c r="J65" t="s">
-        <v>245</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>332</v>
+        <v>260</v>
       </c>
       <c r="B66" t="s">
-        <v>244</v>
-      </c>
-      <c r="C66" t="s">
-        <v>333</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66">
-        <v>2469429</v>
-      </c>
-      <c r="G66" t="s">
-        <v>246</v>
-      </c>
-      <c r="I66">
-        <v>0.66100000000000003</v>
+        <v>188</v>
       </c>
       <c r="J66" t="s">
-        <v>245</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
-      </c>
-      <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67">
-        <v>603</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67">
-        <v>2346901</v>
-      </c>
-      <c r="G67" t="s">
-        <v>60</v>
-      </c>
-      <c r="I67">
-        <v>8.5800000000000001E-2</v>
+        <v>188</v>
       </c>
       <c r="J67" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>273</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68">
-        <v>603</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68">
-        <v>2346901</v>
-      </c>
-      <c r="G68" t="s">
-        <v>60</v>
-      </c>
-      <c r="I68">
-        <v>8.5800000000000001E-2</v>
+        <v>188</v>
       </c>
       <c r="J68" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>364</v>
+        <v>293</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69">
-        <v>603</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69">
-        <v>2346901</v>
-      </c>
-      <c r="G69" t="s">
-        <v>60</v>
-      </c>
-      <c r="I69">
-        <v>8.5800000000000001E-2</v>
+        <v>188</v>
       </c>
       <c r="J69" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>365</v>
+        <v>294</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70">
-        <v>603</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70">
-        <v>2346901</v>
-      </c>
-      <c r="G70" t="s">
-        <v>60</v>
-      </c>
-      <c r="I70">
-        <v>8.5800000000000001E-2</v>
+        <v>188</v>
       </c>
       <c r="J70" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>111</v>
+        <v>295</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71">
-        <v>1084340</v>
-      </c>
-      <c r="G71" t="s">
-        <v>115</v>
-      </c>
-      <c r="H71" t="s">
-        <v>114</v>
-      </c>
-      <c r="I71">
-        <v>0.56499999999999995</v>
+        <v>188</v>
       </c>
       <c r="J71" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
       <c r="B72" t="s">
-        <v>263</v>
+        <v>188</v>
       </c>
       <c r="J72" t="s">
         <v>46</v>
@@ -3009,62 +3666,32 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>198</v>
+        <v>335</v>
       </c>
       <c r="B73" t="s">
-        <v>199</v>
-      </c>
-      <c r="D73">
-        <v>805</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73">
-        <v>7568584</v>
-      </c>
-      <c r="G73" t="s">
-        <v>201</v>
-      </c>
-      <c r="I73">
-        <v>0.22700000000000001</v>
+        <v>188</v>
       </c>
       <c r="J73" t="s">
-        <v>200</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>336</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
-      </c>
-      <c r="D74">
-        <v>805</v>
-      </c>
-      <c r="E74" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74">
-        <v>7568584</v>
-      </c>
-      <c r="G74" t="s">
-        <v>201</v>
-      </c>
-      <c r="I74">
-        <v>0.22700000000000001</v>
+        <v>188</v>
       </c>
       <c r="J74" t="s">
-        <v>200</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>342</v>
       </c>
       <c r="B75" t="s">
-        <v>298</v>
+        <v>188</v>
       </c>
       <c r="J75" t="s">
         <v>46</v>
@@ -3072,46 +3699,43 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>344</v>
       </c>
       <c r="B76" t="s">
-        <v>180</v>
-      </c>
-      <c r="D76" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="J76" t="s">
-        <v>176</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>264</v>
+        <v>346</v>
       </c>
       <c r="B77" t="s">
-        <v>265</v>
+        <v>188</v>
       </c>
       <c r="J77" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>299</v>
+        <v>348</v>
       </c>
       <c r="B78" t="s">
-        <v>265</v>
+        <v>188</v>
       </c>
       <c r="J78" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>350</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="J79" t="s">
         <v>46</v>
@@ -3119,10 +3743,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="J80" t="s">
         <v>46</v>
@@ -3130,1101 +3754,645 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>382</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
-      </c>
-      <c r="C81" t="s">
-        <v>56</v>
-      </c>
-      <c r="D81">
-        <v>1206</v>
-      </c>
-      <c r="E81" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81">
-        <v>1828835</v>
-      </c>
-      <c r="G81" t="s">
-        <v>55</v>
-      </c>
-      <c r="I81">
-        <v>0.154</v>
+        <v>188</v>
       </c>
       <c r="J81" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>386</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
-      </c>
-      <c r="C82" t="s">
-        <v>56</v>
-      </c>
-      <c r="D82">
-        <v>1206</v>
-      </c>
-      <c r="E82" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82">
-        <v>1828835</v>
-      </c>
-      <c r="G82" t="s">
-        <v>55</v>
-      </c>
-      <c r="I82">
-        <v>0.154</v>
+        <v>188</v>
       </c>
       <c r="J82" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>362</v>
+        <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>56</v>
-      </c>
-      <c r="D83">
-        <v>1206</v>
-      </c>
-      <c r="E83" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83">
-        <v>1828835</v>
-      </c>
-      <c r="G83" t="s">
-        <v>55</v>
-      </c>
-      <c r="I83">
-        <v>0.154</v>
+        <v>23</v>
       </c>
       <c r="J83" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>363</v>
+        <v>24</v>
       </c>
       <c r="B84" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>56</v>
-      </c>
-      <c r="D84">
-        <v>1206</v>
-      </c>
-      <c r="E84" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84">
-        <v>1828835</v>
-      </c>
-      <c r="G84" t="s">
-        <v>55</v>
-      </c>
-      <c r="I84">
-        <v>0.154</v>
+        <v>23</v>
       </c>
       <c r="J84" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>45</v>
-      </c>
-      <c r="C85" s="1">
-        <v>1E-3</v>
+        <v>21</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
       </c>
       <c r="J85" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
-      </c>
-      <c r="D86" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="J86" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
-      </c>
-      <c r="D87" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="J87" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>372</v>
+        <v>35</v>
       </c>
       <c r="B88" t="s">
-        <v>373</v>
-      </c>
-      <c r="D88" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="J88" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="B89" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="J89" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>224</v>
+        <v>37</v>
       </c>
       <c r="B90" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="J90" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="J91" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>228</v>
+        <v>68</v>
       </c>
       <c r="B92" t="s">
-        <v>141</v>
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>23</v>
       </c>
       <c r="J92" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>282</v>
+        <v>76</v>
       </c>
       <c r="B93" t="s">
-        <v>141</v>
+        <v>21</v>
+      </c>
+      <c r="C93" t="s">
+        <v>77</v>
       </c>
       <c r="J93" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>369</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>141</v>
+        <v>21</v>
+      </c>
+      <c r="C94" t="s">
+        <v>79</v>
       </c>
       <c r="J94" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="B95" t="s">
-        <v>194</v>
-      </c>
-      <c r="E95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95">
-        <v>1842347</v>
-      </c>
-      <c r="G95" t="s">
-        <v>197</v>
-      </c>
-      <c r="H95" t="s">
-        <v>196</v>
-      </c>
-      <c r="I95">
-        <v>0.58099999999999996</v>
+        <v>21</v>
       </c>
       <c r="J95" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="B96" t="s">
-        <v>63</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96">
-        <v>2061651</v>
-      </c>
-      <c r="G96" t="s">
-        <v>66</v>
-      </c>
-      <c r="H96" t="s">
-        <v>65</v>
-      </c>
-      <c r="I96">
-        <v>0.51200000000000001</v>
+        <v>21</v>
       </c>
       <c r="J96" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>240</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>241</v>
-      </c>
-      <c r="D97" t="s">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="J97" t="s">
-        <v>242</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>338</v>
+        <v>151</v>
       </c>
       <c r="B98" t="s">
-        <v>339</v>
-      </c>
-      <c r="D98" t="s">
-        <v>210</v>
-      </c>
-      <c r="E98" t="s">
-        <v>72</v>
-      </c>
-      <c r="F98" t="s">
-        <v>341</v>
-      </c>
-      <c r="G98" t="s">
-        <v>342</v>
-      </c>
-      <c r="I98">
-        <v>0.16</v>
+        <v>21</v>
       </c>
       <c r="J98" t="s">
-        <v>340</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
       <c r="B99" t="s">
-        <v>205</v>
-      </c>
-      <c r="D99" t="s">
-        <v>210</v>
-      </c>
-      <c r="E99" t="s">
-        <v>72</v>
-      </c>
-      <c r="F99" t="s">
-        <v>208</v>
-      </c>
-      <c r="G99" t="s">
-        <v>209</v>
-      </c>
-      <c r="H99" t="s">
-        <v>207</v>
-      </c>
-      <c r="I99">
-        <v>1.2</v>
+        <v>21</v>
       </c>
       <c r="J99" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="B100" t="s">
-        <v>213</v>
-      </c>
-      <c r="D100" t="s">
-        <v>210</v>
-      </c>
-      <c r="E100" t="s">
-        <v>72</v>
-      </c>
-      <c r="F100" t="s">
-        <v>208</v>
-      </c>
-      <c r="G100" t="s">
-        <v>214</v>
-      </c>
-      <c r="H100" t="s">
-        <v>207</v>
-      </c>
-      <c r="I100">
-        <v>1.2</v>
+        <v>21</v>
       </c>
       <c r="J100" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>69</v>
+        <v>287</v>
       </c>
       <c r="B101" t="s">
-        <v>70</v>
-      </c>
-      <c r="D101" t="s">
-        <v>75</v>
-      </c>
-      <c r="E101" t="s">
-        <v>72</v>
-      </c>
-      <c r="F101" t="s">
-        <v>73</v>
-      </c>
-      <c r="G101" t="s">
-        <v>74</v>
-      </c>
-      <c r="I101">
-        <v>0.48</v>
+        <v>21</v>
       </c>
       <c r="J101" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>248</v>
+        <v>319</v>
       </c>
       <c r="B102" t="s">
-        <v>249</v>
-      </c>
-      <c r="E102" t="s">
-        <v>72</v>
-      </c>
-      <c r="F102" t="s">
-        <v>133</v>
-      </c>
-      <c r="G102" t="s">
-        <v>134</v>
-      </c>
-      <c r="H102" t="s">
-        <v>132</v>
-      </c>
-      <c r="I102">
-        <v>0.22</v>
+        <v>21</v>
       </c>
       <c r="J102" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B103" t="s">
-        <v>251</v>
-      </c>
-      <c r="E103" t="s">
-        <v>72</v>
-      </c>
-      <c r="F103" t="s">
-        <v>133</v>
-      </c>
-      <c r="G103" t="s">
-        <v>134</v>
-      </c>
-      <c r="H103" t="s">
-        <v>132</v>
-      </c>
-      <c r="I103">
-        <v>0.22</v>
+        <v>271</v>
       </c>
       <c r="J103" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
-      </c>
-      <c r="E104" t="s">
-        <v>72</v>
-      </c>
-      <c r="F104" t="s">
-        <v>133</v>
-      </c>
-      <c r="G104" t="s">
-        <v>134</v>
-      </c>
-      <c r="H104" t="s">
-        <v>132</v>
-      </c>
-      <c r="I104">
-        <v>0.22</v>
+        <v>271</v>
       </c>
       <c r="J104" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="B105" t="s">
-        <v>356</v>
-      </c>
-      <c r="D105" t="s">
-        <v>361</v>
-      </c>
-      <c r="E105" t="s">
-        <v>72</v>
-      </c>
-      <c r="F105" t="s">
-        <v>359</v>
-      </c>
-      <c r="G105" t="s">
-        <v>360</v>
-      </c>
-      <c r="H105" t="s">
-        <v>358</v>
-      </c>
-      <c r="I105">
-        <v>0.24</v>
+        <v>271</v>
       </c>
       <c r="J105" t="s">
-        <v>357</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>236</v>
+        <v>381</v>
       </c>
       <c r="B106" t="s">
-        <v>237</v>
-      </c>
-      <c r="D106" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="J106" t="s">
-        <v>238</v>
+        <v>46</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>334</v>
+        <v>136</v>
       </c>
       <c r="B107" t="s">
-        <v>335</v>
-      </c>
-      <c r="C107" t="s">
-        <v>331</v>
+        <v>137</v>
       </c>
       <c r="J107" t="s">
-        <v>330</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" t="s">
-        <v>16</v>
-      </c>
-      <c r="E108" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108">
-        <v>1146032</v>
-      </c>
-      <c r="G108" t="s">
-        <v>15</v>
-      </c>
-      <c r="H108" t="s">
-        <v>13</v>
-      </c>
-      <c r="I108">
-        <v>4.25</v>
+        <v>137</v>
       </c>
       <c r="J108" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>290</v>
+        <v>139</v>
       </c>
       <c r="B109" t="s">
-        <v>291</v>
-      </c>
-      <c r="D109" t="s">
-        <v>293</v>
+        <v>137</v>
       </c>
       <c r="J109" t="s">
-        <v>292</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>253</v>
+        <v>145</v>
       </c>
       <c r="B110" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="J110" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="J111" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B112" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="J112" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B113" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="J113" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="B114" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="J114" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>303</v>
       </c>
       <c r="B115" t="s">
-        <v>165</v>
-      </c>
-      <c r="D115" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="J115" t="s">
-        <v>166</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>168</v>
+        <v>310</v>
       </c>
       <c r="B116" t="s">
-        <v>169</v>
-      </c>
-      <c r="D116" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="J116" t="s">
-        <v>166</v>
+        <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>38</v>
+        <v>316</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
-      </c>
-      <c r="D117" t="s">
-        <v>43</v>
-      </c>
-      <c r="E117" t="s">
-        <v>14</v>
-      </c>
-      <c r="F117">
-        <v>1857299</v>
-      </c>
-      <c r="G117" t="s">
-        <v>42</v>
-      </c>
-      <c r="H117" t="s">
-        <v>41</v>
-      </c>
-      <c r="I117">
-        <v>0.16800000000000001</v>
+        <v>137</v>
       </c>
       <c r="J117" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>211</v>
+        <v>318</v>
       </c>
       <c r="B118" t="s">
-        <v>39</v>
-      </c>
-      <c r="D118" t="s">
-        <v>43</v>
-      </c>
-      <c r="E118" t="s">
-        <v>14</v>
-      </c>
-      <c r="F118">
-        <v>1857299</v>
-      </c>
-      <c r="G118" t="s">
-        <v>42</v>
-      </c>
-      <c r="H118" t="s">
-        <v>41</v>
-      </c>
-      <c r="I118">
-        <v>0.16800000000000001</v>
+        <v>137</v>
       </c>
       <c r="J118" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="B119" t="s">
-        <v>39</v>
-      </c>
-      <c r="D119" t="s">
-        <v>43</v>
-      </c>
-      <c r="E119" t="s">
-        <v>14</v>
-      </c>
-      <c r="F119">
-        <v>1857299</v>
-      </c>
-      <c r="G119" t="s">
-        <v>42</v>
-      </c>
-      <c r="H119" t="s">
-        <v>41</v>
-      </c>
-      <c r="I119">
-        <v>0.16800000000000001</v>
+        <v>137</v>
       </c>
       <c r="J119" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>276</v>
+        <v>389</v>
       </c>
       <c r="B120" t="s">
-        <v>277</v>
-      </c>
-      <c r="D120" t="s">
-        <v>43</v>
-      </c>
-      <c r="E120" t="s">
-        <v>279</v>
-      </c>
-      <c r="F120">
-        <v>1831089</v>
-      </c>
-      <c r="G120" t="s">
-        <v>280</v>
-      </c>
-      <c r="H120" t="s">
-        <v>278</v>
-      </c>
-      <c r="I120">
-        <v>0.224</v>
+        <v>137</v>
       </c>
       <c r="J120" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="B121" t="s">
-        <v>277</v>
-      </c>
-      <c r="D121" t="s">
-        <v>43</v>
-      </c>
-      <c r="E121" t="s">
-        <v>279</v>
-      </c>
-      <c r="F121">
-        <v>1831089</v>
-      </c>
-      <c r="G121" t="s">
-        <v>280</v>
-      </c>
-      <c r="H121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I121">
-        <v>0.224</v>
+        <v>81</v>
+      </c>
+      <c r="C121" t="s">
+        <v>79</v>
       </c>
       <c r="J121" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>318</v>
+        <v>148</v>
       </c>
       <c r="B122" t="s">
-        <v>277</v>
-      </c>
-      <c r="D122" t="s">
-        <v>43</v>
-      </c>
-      <c r="E122" t="s">
-        <v>279</v>
-      </c>
-      <c r="F122">
-        <v>1831089</v>
-      </c>
-      <c r="G122" t="s">
-        <v>280</v>
-      </c>
-      <c r="H122" t="s">
-        <v>278</v>
-      </c>
-      <c r="I122">
-        <v>0.224</v>
+        <v>81</v>
       </c>
       <c r="J122" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="B123" t="s">
-        <v>106</v>
-      </c>
-      <c r="D123" t="s">
-        <v>110</v>
-      </c>
-      <c r="E123" t="s">
-        <v>72</v>
-      </c>
-      <c r="F123" t="s">
-        <v>108</v>
-      </c>
-      <c r="G123" t="s">
-        <v>109</v>
-      </c>
-      <c r="I123">
-        <v>0.12</v>
+        <v>81</v>
       </c>
       <c r="J123" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>328</v>
+        <v>266</v>
       </c>
       <c r="B124" t="s">
-        <v>329</v>
-      </c>
-      <c r="C124" t="s">
-        <v>331</v>
+        <v>267</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J124" t="s">
-        <v>330</v>
+        <v>46</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>374</v>
+        <v>288</v>
       </c>
       <c r="B125" t="s">
-        <v>375</v>
-      </c>
-      <c r="D125" t="s">
-        <v>379</v>
-      </c>
-      <c r="E125" t="s">
-        <v>14</v>
-      </c>
-      <c r="F125">
-        <v>1202826</v>
-      </c>
-      <c r="G125" t="s">
-        <v>378</v>
-      </c>
-      <c r="H125" t="s">
-        <v>377</v>
-      </c>
-      <c r="I125">
-        <v>0.29699999999999999</v>
+        <v>390</v>
+      </c>
+      <c r="C125" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J125" t="s">
-        <v>376</v>
+        <v>46</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="B126" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="J126" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>223</v>
+        <v>144</v>
       </c>
       <c r="B127" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="J127" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="B128" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
       <c r="J128" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>227</v>
+        <v>296</v>
       </c>
       <c r="B129" t="s">
-        <v>18</v>
+        <v>297</v>
       </c>
       <c r="J129" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B130" t="s">
-        <v>18</v>
+        <v>265</v>
       </c>
       <c r="J130" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
       <c r="B131" t="s">
-        <v>18</v>
+        <v>265</v>
       </c>
       <c r="J131" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="B132" t="s">
-        <v>27</v>
-      </c>
-      <c r="C132" t="s">
-        <v>32</v>
-      </c>
-      <c r="D132" t="s">
-        <v>31</v>
-      </c>
-      <c r="E132" t="s">
-        <v>14</v>
-      </c>
-      <c r="F132">
-        <v>1564957</v>
-      </c>
-      <c r="G132" t="s">
-        <v>30</v>
-      </c>
-      <c r="H132" t="s">
-        <v>29</v>
-      </c>
-      <c r="I132">
-        <v>1.33</v>
+        <v>203</v>
       </c>
       <c r="J132" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>229</v>
+        <v>146</v>
       </c>
       <c r="B133" t="s">
-        <v>230</v>
-      </c>
-      <c r="C133" t="s">
-        <v>235</v>
-      </c>
-      <c r="D133" t="s">
-        <v>234</v>
-      </c>
-      <c r="E133" t="s">
-        <v>14</v>
-      </c>
-      <c r="F133">
-        <v>1715855</v>
-      </c>
-      <c r="G133" t="s">
-        <v>233</v>
-      </c>
-      <c r="H133" t="s">
-        <v>232</v>
-      </c>
-      <c r="I133">
-        <v>1.74</v>
+        <v>147</v>
       </c>
       <c r="J133" t="s">
-        <v>231</v>
+        <v>46</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B134" t="s">
-        <v>83</v>
-      </c>
-      <c r="D134" t="s">
-        <v>89</v>
-      </c>
-      <c r="E134" t="s">
-        <v>86</v>
-      </c>
-      <c r="F134" t="s">
-        <v>87</v>
-      </c>
-      <c r="G134" t="s">
-        <v>88</v>
-      </c>
-      <c r="H134" t="s">
-        <v>85</v>
-      </c>
-      <c r="I134">
-        <v>9.58</v>
+        <v>45</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J134" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="B135" t="s">
-        <v>91</v>
-      </c>
-      <c r="D135" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="J135" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="B136" t="s">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="J136" t="s">
         <v>46</v>
@@ -4232,10 +4400,10 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>302</v>
+        <v>226</v>
       </c>
       <c r="B137" t="s">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="J137" t="s">
         <v>46</v>
@@ -4243,10 +4411,10 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>303</v>
+        <v>228</v>
       </c>
       <c r="B138" t="s">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="J138" t="s">
         <v>46</v>
@@ -4254,10 +4422,10 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="B139" t="s">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="J139" t="s">
         <v>46</v>
@@ -4265,10 +4433,10 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>306</v>
+        <v>368</v>
       </c>
       <c r="B140" t="s">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="J140" t="s">
         <v>46</v>
@@ -4276,153 +4444,159 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="B141" t="s">
-        <v>301</v>
+        <v>334</v>
+      </c>
+      <c r="C141" t="s">
+        <v>330</v>
       </c>
       <c r="J141" t="s">
-        <v>22</v>
+        <v>329</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
       <c r="B142" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="J142" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
       <c r="B143" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="J143" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>310</v>
+        <v>257</v>
       </c>
       <c r="B144" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="J144" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="B145" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="J145" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="B146" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="J146" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="B147" t="s">
-        <v>301</v>
+        <v>328</v>
+      </c>
+      <c r="C147" t="s">
+        <v>330</v>
       </c>
       <c r="J147" t="s">
-        <v>22</v>
+        <v>329</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>344</v>
+        <v>17</v>
       </c>
       <c r="B148" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J148" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>346</v>
+        <v>223</v>
       </c>
       <c r="B149" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J149" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>348</v>
+        <v>225</v>
       </c>
       <c r="B150" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J150" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>350</v>
+        <v>227</v>
       </c>
       <c r="B151" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J151" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>352</v>
+        <v>281</v>
       </c>
       <c r="B152" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J152" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="B153" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="J153" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
       <c r="B154" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J154" t="s">
         <v>46</v>
@@ -4430,21 +4604,21 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>367</v>
+        <v>301</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J155" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>370</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J156" t="s">
         <v>46</v>
@@ -4452,43 +4626,43 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>371</v>
+        <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J157" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>380</v>
+        <v>305</v>
       </c>
       <c r="B158" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J158" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>384</v>
+        <v>306</v>
       </c>
       <c r="B159" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J159" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>385</v>
+        <v>307</v>
       </c>
       <c r="B160" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J160" t="s">
         <v>46</v>
@@ -4496,21 +4670,21 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>386</v>
+        <v>308</v>
       </c>
       <c r="B161" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J161" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>388</v>
+        <v>309</v>
       </c>
       <c r="B162" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J162" t="s">
         <v>46</v>
@@ -4518,10 +4692,10 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>389</v>
+        <v>311</v>
       </c>
       <c r="B163" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J163" t="s">
         <v>46</v>
@@ -4529,380 +4703,206 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>181</v>
+        <v>312</v>
       </c>
       <c r="B164" t="s">
-        <v>182</v>
-      </c>
-      <c r="D164" t="s">
-        <v>186</v>
-      </c>
-      <c r="E164" t="s">
-        <v>72</v>
-      </c>
-      <c r="F164" t="s">
-        <v>184</v>
-      </c>
-      <c r="G164" t="s">
-        <v>185</v>
-      </c>
-      <c r="I164">
-        <v>0.63</v>
+        <v>300</v>
       </c>
       <c r="J164" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>101</v>
+        <v>313</v>
       </c>
       <c r="B165" t="s">
-        <v>102</v>
-      </c>
-      <c r="D165" t="s">
-        <v>104</v>
+        <v>300</v>
       </c>
       <c r="J165" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>98</v>
+        <v>343</v>
       </c>
       <c r="B166" t="s">
-        <v>99</v>
-      </c>
-      <c r="D166" t="s">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="J166" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>129</v>
+        <v>345</v>
       </c>
       <c r="B167" t="s">
-        <v>130</v>
-      </c>
-      <c r="E167" t="s">
-        <v>72</v>
-      </c>
-      <c r="F167" t="s">
-        <v>133</v>
-      </c>
-      <c r="G167" t="s">
-        <v>134</v>
-      </c>
-      <c r="H167" t="s">
-        <v>132</v>
-      </c>
-      <c r="I167">
-        <v>0.22</v>
+        <v>300</v>
       </c>
       <c r="J167" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>117</v>
+        <v>347</v>
       </c>
       <c r="B168" t="s">
-        <v>118</v>
-      </c>
-      <c r="D168" t="s">
-        <v>122</v>
-      </c>
-      <c r="E168" t="s">
-        <v>72</v>
-      </c>
-      <c r="F168" t="s">
-        <v>120</v>
-      </c>
-      <c r="G168" t="s">
-        <v>121</v>
-      </c>
-      <c r="I168">
-        <v>0.09</v>
+        <v>300</v>
       </c>
       <c r="J168" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>94</v>
+        <v>349</v>
       </c>
       <c r="B169" t="s">
-        <v>95</v>
-      </c>
-      <c r="D169" t="s">
-        <v>97</v>
+        <v>300</v>
       </c>
       <c r="J169" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>215</v>
+        <v>351</v>
       </c>
       <c r="B170" t="s">
-        <v>216</v>
-      </c>
-      <c r="D170" t="s">
-        <v>220</v>
-      </c>
-      <c r="E170" t="s">
-        <v>72</v>
-      </c>
-      <c r="F170" t="s">
-        <v>218</v>
-      </c>
-      <c r="G170" t="s">
-        <v>219</v>
-      </c>
-      <c r="I170">
-        <v>0.12</v>
+        <v>300</v>
       </c>
       <c r="J170" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>221</v>
+        <v>353</v>
       </c>
       <c r="B171" t="s">
-        <v>222</v>
-      </c>
-      <c r="D171" t="s">
-        <v>220</v>
-      </c>
-      <c r="E171" t="s">
-        <v>72</v>
-      </c>
-      <c r="F171" t="s">
-        <v>218</v>
-      </c>
-      <c r="G171" t="s">
-        <v>219</v>
-      </c>
-      <c r="I171">
-        <v>0.12</v>
+        <v>300</v>
       </c>
       <c r="J171" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>158</v>
+        <v>365</v>
       </c>
       <c r="B172" t="s">
-        <v>159</v>
-      </c>
-      <c r="E172" t="s">
-        <v>86</v>
-      </c>
-      <c r="F172" t="s">
-        <v>162</v>
-      </c>
-      <c r="G172" t="s">
-        <v>163</v>
-      </c>
-      <c r="H172" t="s">
-        <v>161</v>
-      </c>
-      <c r="I172">
-        <v>7.39</v>
+        <v>300</v>
       </c>
       <c r="J172" t="s">
-        <v>160</v>
+        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>321</v>
+        <v>366</v>
       </c>
       <c r="B173" t="s">
-        <v>322</v>
-      </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173">
-        <v>1772204</v>
-      </c>
-      <c r="G173" t="s">
-        <v>325</v>
-      </c>
-      <c r="H173" t="s">
-        <v>324</v>
-      </c>
-      <c r="I173">
-        <v>56.5</v>
+        <v>300</v>
       </c>
       <c r="J173" t="s">
-        <v>323</v>
+        <v>22</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>154</v>
+        <v>369</v>
       </c>
       <c r="B174" t="s">
-        <v>155</v>
-      </c>
-      <c r="D174" t="s">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="J174" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>191</v>
+        <v>370</v>
       </c>
       <c r="B175" t="s">
-        <v>192</v>
-      </c>
-      <c r="D175" t="s">
-        <v>97</v>
+        <v>300</v>
       </c>
       <c r="J175" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>156</v>
+        <v>379</v>
       </c>
       <c r="B176" t="s">
-        <v>157</v>
-      </c>
-      <c r="D176" t="s">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="J176" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>189</v>
+        <v>383</v>
       </c>
       <c r="B177" t="s">
-        <v>190</v>
-      </c>
-      <c r="D177" t="s">
-        <v>97</v>
+        <v>300</v>
       </c>
       <c r="J177" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>47</v>
+        <v>384</v>
       </c>
       <c r="B178" t="s">
-        <v>48</v>
-      </c>
-      <c r="E178" t="s">
-        <v>14</v>
-      </c>
-      <c r="F178">
-        <v>1696320</v>
-      </c>
-      <c r="G178" t="s">
-        <v>51</v>
-      </c>
-      <c r="H178" t="s">
-        <v>50</v>
-      </c>
-      <c r="I178">
-        <v>4.4000000000000004</v>
+        <v>300</v>
       </c>
       <c r="J178" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>315</v>
+        <v>385</v>
       </c>
       <c r="B179" t="s">
-        <v>48</v>
-      </c>
-      <c r="E179" t="s">
-        <v>14</v>
-      </c>
-      <c r="F179">
-        <v>1696320</v>
-      </c>
-      <c r="G179" t="s">
-        <v>51</v>
-      </c>
-      <c r="H179" t="s">
-        <v>50</v>
-      </c>
-      <c r="I179">
-        <v>4.4000000000000004</v>
+        <v>300</v>
       </c>
       <c r="J179" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>170</v>
+        <v>387</v>
       </c>
       <c r="B180" t="s">
-        <v>171</v>
-      </c>
-      <c r="D180" t="s">
-        <v>173</v>
+        <v>300</v>
       </c>
       <c r="J180" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>123</v>
+        <v>388</v>
       </c>
       <c r="B181" t="s">
-        <v>124</v>
-      </c>
-      <c r="E181" t="s">
-        <v>72</v>
-      </c>
-      <c r="F181" t="s">
-        <v>127</v>
-      </c>
-      <c r="G181" t="s">
-        <v>128</v>
-      </c>
-      <c r="H181" t="s">
-        <v>126</v>
-      </c>
-      <c r="I181">
-        <v>0.26</v>
+        <v>300</v>
       </c>
       <c r="J181" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">
     <sortState ref="A2:J181">
-      <sortCondition ref="B1"/>
+      <sortCondition ref="F1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Wert von R3 von 0R auf n.B. geändert
</commit_message>
<xml_diff>
--- a/kicad_ucboard/ucboard_Teileliste.xlsx
+++ b/kicad_ucboard/ucboard_Teileliste.xlsx
@@ -2038,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2081,236 +2081,176 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>362</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>116</v>
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>1206</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2">
-        <v>1084340</v>
+        <v>1828835</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="I2">
-        <v>0.56499999999999995</v>
+        <v>0.154</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>1146032</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3">
-        <v>4.25</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>373</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>374</v>
-      </c>
-      <c r="D4" t="s">
-        <v>378</v>
+        <v>199</v>
+      </c>
+      <c r="D4">
+        <v>805</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4">
-        <v>1202826</v>
+        <v>7568584</v>
       </c>
       <c r="G4" t="s">
-        <v>377</v>
-      </c>
-      <c r="H4" t="s">
-        <v>376</v>
+        <v>201</v>
       </c>
       <c r="I4">
-        <v>0.29699999999999999</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="J4" t="s">
-        <v>375</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
+        <v>199</v>
+      </c>
+      <c r="D5">
+        <v>805</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5">
-        <v>1564957</v>
+        <v>7568584</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
       <c r="I5">
-        <v>1.33</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>287</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>1696320</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6">
-        <v>4.4000000000000004</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>314</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>247</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7">
-        <v>1696320</v>
+        <v>2469429</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
+        <v>246</v>
       </c>
       <c r="I7">
-        <v>4.4000000000000004</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
-      </c>
-      <c r="C8" t="s">
-        <v>235</v>
-      </c>
-      <c r="D8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8">
-        <v>1715855</v>
-      </c>
-      <c r="G8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I8">
-        <v>1.74</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>231</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>321</v>
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>1206</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9">
-        <v>1772204</v>
+        <v>1828835</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H9" t="s">
-        <v>323</v>
+        <v>55</v>
       </c>
       <c r="I9">
-        <v>56.5</v>
+        <v>0.154</v>
       </c>
       <c r="J9" t="s">
-        <v>322</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
@@ -2339,341 +2279,203 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11">
-        <v>1206</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11">
-        <v>1828835</v>
-      </c>
-      <c r="G11" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11">
-        <v>0.154</v>
+        <v>300</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>361</v>
+        <v>284</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12">
-        <v>1206</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12">
-        <v>1828835</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12">
-        <v>0.154</v>
+        <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D13">
-        <v>1206</v>
+        <v>603</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13">
-        <v>1828835</v>
+        <v>2346901</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I13">
-        <v>0.154</v>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>603</v>
       </c>
       <c r="E14" t="s">
-        <v>279</v>
+        <v>14</v>
       </c>
       <c r="F14">
-        <v>1831089</v>
+        <v>2346901</v>
       </c>
       <c r="G14" t="s">
-        <v>280</v>
-      </c>
-      <c r="H14" t="s">
-        <v>278</v>
+        <v>60</v>
       </c>
       <c r="I14">
-        <v>0.224</v>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
-        <v>277</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>279</v>
-      </c>
-      <c r="F15">
-        <v>1831089</v>
-      </c>
-      <c r="G15" t="s">
-        <v>280</v>
-      </c>
-      <c r="H15" t="s">
-        <v>278</v>
-      </c>
-      <c r="I15">
-        <v>0.224</v>
+        <v>265</v>
       </c>
       <c r="J15" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
+        <v>244</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
       </c>
       <c r="E16" t="s">
-        <v>279</v>
+        <v>14</v>
       </c>
       <c r="F16">
-        <v>1831089</v>
+        <v>2469429</v>
       </c>
       <c r="G16" t="s">
-        <v>280</v>
-      </c>
-      <c r="H16" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="I16">
-        <v>0.224</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>603</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
       </c>
       <c r="F17">
-        <v>1842347</v>
+        <v>2346901</v>
       </c>
       <c r="G17" t="s">
-        <v>197</v>
-      </c>
-      <c r="H17" t="s">
-        <v>196</v>
+        <v>60</v>
       </c>
       <c r="I17">
-        <v>0.58099999999999996</v>
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J17" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18">
-        <v>1857299</v>
-      </c>
-      <c r="G18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18">
-        <v>0.16800000000000001</v>
+        <v>265</v>
       </c>
       <c r="J18" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>313</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19">
-        <v>1857299</v>
-      </c>
-      <c r="G19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19">
-        <v>0.16800000000000001</v>
+        <v>300</v>
       </c>
       <c r="J19" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>315</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20">
-        <v>1857299</v>
-      </c>
-      <c r="G20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20">
-        <v>0.16800000000000001</v>
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21">
-        <v>2061651</v>
-      </c>
-      <c r="G21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21">
-        <v>0.51200000000000001</v>
+        <v>21</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22">
-        <v>603</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22">
-        <v>2346901</v>
-      </c>
-      <c r="G22" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22">
-        <v>8.5800000000000001E-2</v>
+        <v>21</v>
       </c>
       <c r="J22" t="s">
         <v>22</v>
@@ -2681,28 +2483,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23">
-        <v>603</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23">
-        <v>2346901</v>
-      </c>
-      <c r="G23" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23">
-        <v>8.5800000000000001E-2</v>
+        <v>79</v>
       </c>
       <c r="J23" t="s">
         <v>22</v>
@@ -2710,28 +2497,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>363</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24">
-        <v>603</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24">
-        <v>2346901</v>
-      </c>
-      <c r="G24" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24">
-        <v>8.5800000000000001E-2</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
@@ -2739,28 +2508,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>364</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25">
-        <v>603</v>
-      </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25">
-        <v>2346901</v>
-      </c>
-      <c r="G25" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25">
-        <v>8.5800000000000001E-2</v>
+        <v>79</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
@@ -2768,1256 +2522,1280 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>244</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>247</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26">
-        <v>2469429</v>
-      </c>
-      <c r="G26" t="s">
-        <v>246</v>
-      </c>
-      <c r="I26">
-        <v>0.66100000000000003</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>331</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
-      </c>
-      <c r="C27" t="s">
-        <v>332</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27">
-        <v>2469429</v>
-      </c>
-      <c r="G27" t="s">
-        <v>246</v>
-      </c>
-      <c r="I27">
-        <v>0.66100000000000003</v>
+        <v>21</v>
       </c>
       <c r="J27" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
-      </c>
-      <c r="D28">
-        <v>805</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28">
-        <v>7568584</v>
-      </c>
-      <c r="G28" t="s">
-        <v>201</v>
-      </c>
-      <c r="I28">
-        <v>0.22700000000000001</v>
+        <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>200</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>252</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29">
-        <v>805</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29">
-        <v>7568584</v>
-      </c>
-      <c r="G29" t="s">
-        <v>201</v>
-      </c>
-      <c r="I29">
-        <v>0.22700000000000001</v>
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
       </c>
       <c r="J29" t="s">
-        <v>200</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H30" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30">
-        <v>9.58</v>
+        <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
-      </c>
-      <c r="E31" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" t="s">
-        <v>162</v>
-      </c>
-      <c r="G31" t="s">
-        <v>163</v>
-      </c>
-      <c r="H31" t="s">
-        <v>161</v>
-      </c>
-      <c r="I31">
-        <v>7.39</v>
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
       </c>
       <c r="J31" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B32" t="s">
-        <v>355</v>
-      </c>
-      <c r="D32" t="s">
-        <v>360</v>
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32">
+        <v>1206</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" t="s">
-        <v>358</v>
+        <v>14</v>
+      </c>
+      <c r="F32">
+        <v>1828835</v>
       </c>
       <c r="G32" t="s">
-        <v>359</v>
-      </c>
-      <c r="H32" t="s">
-        <v>357</v>
+        <v>55</v>
       </c>
       <c r="I32">
-        <v>0.24</v>
+        <v>0.154</v>
       </c>
       <c r="J32" t="s">
-        <v>356</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
-      </c>
-      <c r="I33">
-        <v>0.48</v>
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
       </c>
       <c r="J33" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
-      </c>
-      <c r="D34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" t="s">
-        <v>184</v>
-      </c>
-      <c r="G34" t="s">
-        <v>185</v>
-      </c>
-      <c r="I34">
-        <v>0.63</v>
+        <v>21</v>
       </c>
       <c r="J34" t="s">
-        <v>183</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>153</v>
       </c>
       <c r="B35" t="s">
-        <v>249</v>
-      </c>
-      <c r="E35" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" t="s">
-        <v>133</v>
-      </c>
-      <c r="G35" t="s">
-        <v>134</v>
-      </c>
-      <c r="H35" t="s">
-        <v>132</v>
-      </c>
-      <c r="I35">
-        <v>0.22</v>
+        <v>81</v>
       </c>
       <c r="J35" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>250</v>
+        <v>343</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
-      </c>
-      <c r="E36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" t="s">
-        <v>132</v>
-      </c>
-      <c r="I36">
-        <v>0.22</v>
+        <v>300</v>
       </c>
       <c r="J36" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B37" t="s">
-        <v>259</v>
-      </c>
-      <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>133</v>
-      </c>
-      <c r="G37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H37" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37">
-        <v>0.22</v>
+        <v>300</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>347</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" t="s">
-        <v>133</v>
-      </c>
-      <c r="G38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38">
-        <v>0.22</v>
+        <v>300</v>
       </c>
       <c r="J38" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>351</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
-      </c>
-      <c r="E39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" t="s">
-        <v>128</v>
-      </c>
-      <c r="H39" t="s">
-        <v>126</v>
-      </c>
-      <c r="I39">
-        <v>0.26</v>
+        <v>300</v>
       </c>
       <c r="J39" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>349</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
-      </c>
-      <c r="D40" t="s">
-        <v>210</v>
-      </c>
-      <c r="E40" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" t="s">
-        <v>208</v>
-      </c>
-      <c r="G40" t="s">
-        <v>209</v>
-      </c>
-      <c r="H40" t="s">
-        <v>207</v>
-      </c>
-      <c r="I40">
-        <v>1.2</v>
+        <v>300</v>
       </c>
       <c r="J40" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>353</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" t="s">
-        <v>210</v>
-      </c>
-      <c r="E41" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" t="s">
-        <v>208</v>
-      </c>
-      <c r="G41" t="s">
-        <v>214</v>
-      </c>
-      <c r="H41" t="s">
-        <v>207</v>
-      </c>
-      <c r="I41">
-        <v>1.2</v>
+        <v>300</v>
       </c>
       <c r="J41" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>366</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" t="s">
-        <v>122</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" t="s">
-        <v>120</v>
-      </c>
-      <c r="G42" t="s">
-        <v>121</v>
-      </c>
-      <c r="I42">
-        <v>0.09</v>
+        <v>300</v>
       </c>
       <c r="J42" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>215</v>
+        <v>370</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" t="s">
-        <v>220</v>
-      </c>
-      <c r="E43" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" t="s">
-        <v>218</v>
-      </c>
-      <c r="G43" t="s">
-        <v>219</v>
-      </c>
-      <c r="I43">
-        <v>0.12</v>
+        <v>300</v>
       </c>
       <c r="J43" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>221</v>
+        <v>385</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
-      </c>
-      <c r="D44" t="s">
-        <v>220</v>
-      </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" t="s">
-        <v>218</v>
-      </c>
-      <c r="G44" t="s">
-        <v>219</v>
-      </c>
-      <c r="I44">
-        <v>0.12</v>
+        <v>300</v>
       </c>
       <c r="J44" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45" t="s">
-        <v>110</v>
-      </c>
-      <c r="E45" t="s">
-        <v>72</v>
-      </c>
-      <c r="F45" t="s">
-        <v>108</v>
-      </c>
-      <c r="G45" t="s">
-        <v>109</v>
-      </c>
-      <c r="I45">
-        <v>0.12</v>
+        <v>21</v>
       </c>
       <c r="J45" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
-      </c>
-      <c r="D46" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" t="s">
-        <v>340</v>
-      </c>
-      <c r="G46" t="s">
-        <v>341</v>
-      </c>
-      <c r="I46">
-        <v>0.16</v>
+        <v>300</v>
       </c>
       <c r="J46" t="s">
-        <v>339</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>364</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" t="s">
-        <v>104</v>
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47">
+        <v>603</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47">
+        <v>2346901</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="I47">
+        <v>8.5800000000000001E-2</v>
       </c>
       <c r="J47" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="J48" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J49" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="J50" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B51" t="s">
-        <v>290</v>
-      </c>
-      <c r="D51" t="s">
-        <v>292</v>
+        <v>18</v>
       </c>
       <c r="J51" t="s">
-        <v>291</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="J52" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s">
-        <v>192</v>
-      </c>
-      <c r="D53" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="J53" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="B54" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="J54" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="J55" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>179</v>
+        <v>367</v>
       </c>
       <c r="B56" t="s">
-        <v>180</v>
-      </c>
-      <c r="D56" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="J56" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>177</v>
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57">
+        <v>1146032</v>
+      </c>
+      <c r="G57" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57">
+        <v>4.25</v>
       </c>
       <c r="J57" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
-      </c>
-      <c r="D58" t="s">
-        <v>177</v>
+        <v>63</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58">
+        <v>2061651</v>
+      </c>
+      <c r="G58" t="s">
+        <v>66</v>
+      </c>
+      <c r="H58" t="s">
+        <v>65</v>
+      </c>
+      <c r="I58">
+        <v>0.51200000000000001</v>
       </c>
       <c r="J58" t="s">
-        <v>176</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="B59" t="s">
-        <v>372</v>
-      </c>
-      <c r="D59" t="s">
-        <v>177</v>
+        <v>328</v>
+      </c>
+      <c r="C59" t="s">
+        <v>330</v>
       </c>
       <c r="J59" t="s">
-        <v>176</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>170</v>
+        <v>333</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
-      </c>
-      <c r="D60" t="s">
-        <v>173</v>
+        <v>334</v>
+      </c>
+      <c r="C60" t="s">
+        <v>330</v>
       </c>
       <c r="J60" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B61" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D61" t="s">
-        <v>167</v>
+        <v>186</v>
+      </c>
+      <c r="E61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" t="s">
+        <v>184</v>
+      </c>
+      <c r="G61" t="s">
+        <v>185</v>
+      </c>
+      <c r="I61">
+        <v>0.63</v>
       </c>
       <c r="J61" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>169</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>167</v>
+        <v>75</v>
+      </c>
+      <c r="E62" t="s">
+        <v>72</v>
+      </c>
+      <c r="F62" t="s">
+        <v>73</v>
+      </c>
+      <c r="G62" t="s">
+        <v>74</v>
+      </c>
+      <c r="I62">
+        <v>0.48</v>
       </c>
       <c r="J62" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
       <c r="B63" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
       <c r="D63" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="J63" t="s">
-        <v>242</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>239</v>
+        <v>97</v>
       </c>
       <c r="J64" t="s">
-        <v>238</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>124</v>
+      </c>
+      <c r="E65" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G65" t="s">
+        <v>128</v>
+      </c>
+      <c r="H65" t="s">
+        <v>126</v>
+      </c>
+      <c r="I65">
+        <v>0.26</v>
       </c>
       <c r="J65" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>260</v>
+        <v>354</v>
       </c>
       <c r="B66" t="s">
-        <v>188</v>
+        <v>355</v>
+      </c>
+      <c r="D66" t="s">
+        <v>360</v>
+      </c>
+      <c r="E66" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" t="s">
+        <v>358</v>
+      </c>
+      <c r="G66" t="s">
+        <v>359</v>
+      </c>
+      <c r="H66" t="s">
+        <v>357</v>
+      </c>
+      <c r="I66">
+        <v>0.24</v>
       </c>
       <c r="J66" t="s">
-        <v>46</v>
+        <v>356</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>261</v>
+        <v>105</v>
       </c>
       <c r="B67" t="s">
-        <v>188</v>
+        <v>106</v>
+      </c>
+      <c r="D67" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" t="s">
+        <v>108</v>
+      </c>
+      <c r="G67" t="s">
+        <v>109</v>
+      </c>
+      <c r="I67">
+        <v>0.12</v>
       </c>
       <c r="J67" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>237</v>
+      </c>
+      <c r="D68" t="s">
+        <v>239</v>
       </c>
       <c r="J68" t="s">
-        <v>46</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>293</v>
+        <v>240</v>
       </c>
       <c r="B69" t="s">
-        <v>188</v>
+        <v>241</v>
+      </c>
+      <c r="D69" t="s">
+        <v>122</v>
       </c>
       <c r="J69" t="s">
-        <v>46</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>294</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>188</v>
+        <v>91</v>
+      </c>
+      <c r="D70" t="s">
+        <v>93</v>
       </c>
       <c r="J70" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>295</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>95</v>
+      </c>
+      <c r="D71" t="s">
+        <v>97</v>
       </c>
       <c r="J71" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>326</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>188</v>
+        <v>99</v>
+      </c>
+      <c r="D72" t="s">
+        <v>75</v>
       </c>
       <c r="J72" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>335</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>188</v>
+        <v>165</v>
+      </c>
+      <c r="D73" t="s">
+        <v>167</v>
       </c>
       <c r="J73" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>336</v>
+        <v>168</v>
       </c>
       <c r="B74" t="s">
-        <v>188</v>
+        <v>169</v>
+      </c>
+      <c r="D74" t="s">
+        <v>167</v>
       </c>
       <c r="J74" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>342</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>118</v>
+      </c>
+      <c r="D75" t="s">
+        <v>122</v>
+      </c>
+      <c r="E75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" t="s">
+        <v>120</v>
+      </c>
+      <c r="G75" t="s">
+        <v>121</v>
+      </c>
+      <c r="I75">
+        <v>0.09</v>
       </c>
       <c r="J75" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>344</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>175</v>
+      </c>
+      <c r="D76" t="s">
+        <v>177</v>
       </c>
       <c r="J76" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>346</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
+        <v>175</v>
+      </c>
+      <c r="D77" t="s">
+        <v>177</v>
       </c>
       <c r="J77" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>348</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>180</v>
+      </c>
+      <c r="D78" t="s">
+        <v>177</v>
       </c>
       <c r="J78" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>350</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
+        <v>171</v>
+      </c>
+      <c r="D79" t="s">
+        <v>173</v>
       </c>
       <c r="J79" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>352</v>
+        <v>215</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>216</v>
+      </c>
+      <c r="D80" t="s">
+        <v>220</v>
+      </c>
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+      <c r="F80" t="s">
+        <v>218</v>
+      </c>
+      <c r="G80" t="s">
+        <v>219</v>
+      </c>
+      <c r="I80">
+        <v>0.12</v>
       </c>
       <c r="J80" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>382</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>222</v>
+      </c>
+      <c r="D81" t="s">
+        <v>220</v>
+      </c>
+      <c r="E81" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81" t="s">
+        <v>218</v>
+      </c>
+      <c r="G81" t="s">
+        <v>219</v>
+      </c>
+      <c r="I81">
+        <v>0.12</v>
       </c>
       <c r="J81" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="B82" t="s">
-        <v>188</v>
+        <v>372</v>
+      </c>
+      <c r="D82" t="s">
+        <v>177</v>
       </c>
       <c r="J82" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
-      </c>
-      <c r="C83" t="s">
-        <v>23</v>
+        <v>102</v>
+      </c>
+      <c r="D83" t="s">
+        <v>104</v>
       </c>
       <c r="J83" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>204</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" t="s">
-        <v>23</v>
+        <v>205</v>
+      </c>
+      <c r="D84" t="s">
+        <v>210</v>
+      </c>
+      <c r="E84" t="s">
+        <v>72</v>
+      </c>
+      <c r="F84" t="s">
+        <v>208</v>
+      </c>
+      <c r="G84" t="s">
+        <v>209</v>
+      </c>
+      <c r="H84" t="s">
+        <v>207</v>
+      </c>
+      <c r="I84">
+        <v>1.2</v>
       </c>
       <c r="J84" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>337</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s">
-        <v>23</v>
+        <v>338</v>
+      </c>
+      <c r="D85" t="s">
+        <v>210</v>
+      </c>
+      <c r="E85" t="s">
+        <v>72</v>
+      </c>
+      <c r="F85" t="s">
+        <v>340</v>
+      </c>
+      <c r="G85" t="s">
+        <v>341</v>
+      </c>
+      <c r="I85">
+        <v>0.16</v>
       </c>
       <c r="J85" t="s">
-        <v>22</v>
+        <v>339</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>33</v>
+        <v>212</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>213</v>
+      </c>
+      <c r="D86" t="s">
+        <v>210</v>
+      </c>
+      <c r="E86" t="s">
+        <v>72</v>
+      </c>
+      <c r="F86" t="s">
+        <v>208</v>
+      </c>
+      <c r="G86" t="s">
+        <v>214</v>
+      </c>
+      <c r="H86" t="s">
+        <v>207</v>
+      </c>
+      <c r="I86">
+        <v>1.2</v>
       </c>
       <c r="J86" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>155</v>
+      </c>
+      <c r="D87" t="s">
+        <v>75</v>
       </c>
       <c r="J87" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>157</v>
+      </c>
+      <c r="D88" t="s">
+        <v>75</v>
       </c>
       <c r="J88" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>36</v>
+        <v>289</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>290</v>
+      </c>
+      <c r="D89" t="s">
+        <v>292</v>
       </c>
       <c r="J89" t="s">
-        <v>22</v>
+        <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>37</v>
+        <v>253</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="J90" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>57</v>
+        <v>256</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="J91" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" t="s">
-        <v>23</v>
+        <v>254</v>
       </c>
       <c r="J92" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>274</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" t="s">
-        <v>77</v>
+        <v>254</v>
       </c>
       <c r="J93" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>78</v>
+        <v>275</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
-      </c>
-      <c r="C94" t="s">
-        <v>79</v>
+        <v>254</v>
       </c>
       <c r="J94" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>277</v>
+      </c>
+      <c r="D95" t="s">
+        <v>43</v>
+      </c>
+      <c r="E95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F95">
+        <v>1831089</v>
+      </c>
+      <c r="G95" t="s">
+        <v>280</v>
+      </c>
+      <c r="H95" t="s">
+        <v>278</v>
+      </c>
+      <c r="I95">
+        <v>0.224</v>
       </c>
       <c r="J95" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>149</v>
+        <v>315</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="D96" t="s">
+        <v>43</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96">
+        <v>1857299</v>
+      </c>
+      <c r="G96" t="s">
+        <v>42</v>
+      </c>
+      <c r="H96" t="s">
+        <v>41</v>
+      </c>
+      <c r="I96">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J96" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="D97" t="s">
+        <v>43</v>
+      </c>
+      <c r="E97" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97">
+        <v>1857299</v>
+      </c>
+      <c r="G97" t="s">
+        <v>42</v>
+      </c>
+      <c r="H97" t="s">
+        <v>41</v>
+      </c>
+      <c r="I97">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J97" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>317</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>277</v>
+      </c>
+      <c r="D98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E98" t="s">
+        <v>279</v>
+      </c>
+      <c r="F98">
+        <v>1831089</v>
+      </c>
+      <c r="G98" t="s">
+        <v>280</v>
+      </c>
+      <c r="H98" t="s">
+        <v>278</v>
+      </c>
+      <c r="I98">
+        <v>0.224</v>
       </c>
       <c r="J98" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>152</v>
+        <v>276</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>277</v>
+      </c>
+      <c r="D99" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" t="s">
+        <v>279</v>
+      </c>
+      <c r="F99">
+        <v>1831089</v>
+      </c>
+      <c r="G99" t="s">
+        <v>280</v>
+      </c>
+      <c r="H99" t="s">
+        <v>278</v>
+      </c>
+      <c r="I99">
+        <v>0.224</v>
       </c>
       <c r="J99" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>284</v>
+        <v>211</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
+        <v>43</v>
+      </c>
+      <c r="E100" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100">
+        <v>1857299</v>
+      </c>
+      <c r="G100" t="s">
+        <v>42</v>
+      </c>
+      <c r="H100" t="s">
+        <v>41</v>
+      </c>
+      <c r="I100">
+        <v>0.16800000000000001</v>
       </c>
       <c r="J100" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
+        <v>188</v>
       </c>
       <c r="J101" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>319</v>
+        <v>272</v>
       </c>
       <c r="B102" t="s">
-        <v>21</v>
+        <v>271</v>
       </c>
       <c r="J102" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B103" t="s">
-        <v>271</v>
+        <v>137</v>
       </c>
       <c r="J103" t="s">
         <v>46</v>
@@ -4025,10 +3803,10 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>272</v>
+        <v>318</v>
       </c>
       <c r="B104" t="s">
-        <v>271</v>
+        <v>137</v>
       </c>
       <c r="J104" t="s">
         <v>46</v>
@@ -4036,10 +3814,10 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>380</v>
+        <v>268</v>
       </c>
       <c r="B105" t="s">
-        <v>271</v>
+        <v>137</v>
       </c>
       <c r="J105" t="s">
         <v>46</v>
@@ -4047,10 +3825,10 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>381</v>
+        <v>325</v>
       </c>
       <c r="B106" t="s">
-        <v>271</v>
+        <v>137</v>
       </c>
       <c r="J106" t="s">
         <v>46</v>
@@ -4058,10 +3836,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>365</v>
       </c>
       <c r="B107" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J107" t="s">
         <v>46</v>
@@ -4069,10 +3847,10 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>304</v>
       </c>
       <c r="B108" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J108" t="s">
         <v>46</v>
@@ -4080,7 +3858,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>139</v>
+        <v>303</v>
       </c>
       <c r="B109" t="s">
         <v>137</v>
@@ -4091,10 +3869,10 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="B110" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="J110" t="s">
         <v>46</v>
@@ -4102,10 +3880,10 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>268</v>
+        <v>305</v>
       </c>
       <c r="B111" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J111" t="s">
         <v>46</v>
@@ -4113,10 +3891,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>269</v>
+        <v>202</v>
       </c>
       <c r="B112" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="J112" t="s">
         <v>46</v>
@@ -4124,10 +3902,10 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="B113" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="J113" t="s">
         <v>46</v>
@@ -4135,10 +3913,10 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="B114" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J114" t="s">
         <v>46</v>
@@ -4146,10 +3924,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B115" t="s">
-        <v>137</v>
+        <v>390</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J115" t="s">
         <v>46</v>
@@ -4157,10 +3938,13 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="B116" t="s">
-        <v>137</v>
+        <v>267</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J116" t="s">
         <v>46</v>
@@ -4168,10 +3952,10 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B117" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J117" t="s">
         <v>46</v>
@@ -4179,7 +3963,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="B118" t="s">
         <v>137</v>
@@ -4190,10 +3974,10 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>325</v>
+        <v>383</v>
       </c>
       <c r="B119" t="s">
-        <v>137</v>
+        <v>300</v>
       </c>
       <c r="J119" t="s">
         <v>46</v>
@@ -4201,7 +3985,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>389</v>
+        <v>269</v>
       </c>
       <c r="B120" t="s">
         <v>137</v>
@@ -4212,49 +3996,43 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>80</v>
+        <v>299</v>
       </c>
       <c r="B121" t="s">
-        <v>81</v>
-      </c>
-      <c r="C121" t="s">
-        <v>79</v>
+        <v>300</v>
       </c>
       <c r="J121" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="B122" t="s">
-        <v>81</v>
+        <v>263</v>
       </c>
       <c r="J122" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>153</v>
+        <v>260</v>
       </c>
       <c r="B123" t="s">
-        <v>81</v>
+        <v>300</v>
       </c>
       <c r="J123" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="B124" t="s">
-        <v>267</v>
-      </c>
-      <c r="C124" s="1">
-        <v>1E-3</v>
+        <v>300</v>
       </c>
       <c r="J124" t="s">
         <v>46</v>
@@ -4262,13 +4040,10 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="B125" t="s">
-        <v>390</v>
-      </c>
-      <c r="C125" s="1">
-        <v>1E-3</v>
+        <v>137</v>
       </c>
       <c r="J125" t="s">
         <v>46</v>
@@ -4276,10 +4051,10 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>142</v>
+        <v>296</v>
       </c>
       <c r="B126" t="s">
-        <v>143</v>
+        <v>297</v>
       </c>
       <c r="J126" t="s">
         <v>46</v>
@@ -4287,10 +4062,10 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="B127" t="s">
-        <v>143</v>
+        <v>300</v>
       </c>
       <c r="J127" t="s">
         <v>46</v>
@@ -4298,10 +4073,10 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="B128" t="s">
-        <v>263</v>
+        <v>300</v>
       </c>
       <c r="J128" t="s">
         <v>46</v>
@@ -4309,10 +4084,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="J129" t="s">
         <v>46</v>
@@ -4320,32 +4095,32 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>264</v>
+        <v>384</v>
       </c>
       <c r="B130" t="s">
-        <v>265</v>
+        <v>300</v>
       </c>
       <c r="J130" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B131" t="s">
-        <v>265</v>
+        <v>300</v>
       </c>
       <c r="J131" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>202</v>
+        <v>136</v>
       </c>
       <c r="B132" t="s">
-        <v>203</v>
+        <v>137</v>
       </c>
       <c r="J132" t="s">
         <v>46</v>
@@ -4353,10 +4128,10 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B133" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J133" t="s">
         <v>46</v>
@@ -4364,13 +4139,10 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>44</v>
+        <v>316</v>
       </c>
       <c r="B134" t="s">
-        <v>45</v>
-      </c>
-      <c r="C134" s="1">
-        <v>1E-3</v>
+        <v>137</v>
       </c>
       <c r="J134" t="s">
         <v>46</v>
@@ -4378,10 +4150,10 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J135" t="s">
         <v>46</v>
@@ -4389,10 +4161,10 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>224</v>
+        <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="J136" t="s">
         <v>46</v>
@@ -4400,10 +4172,10 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>226</v>
+        <v>145</v>
       </c>
       <c r="B137" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J137" t="s">
         <v>46</v>
@@ -4411,7 +4183,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B138" t="s">
         <v>141</v>
@@ -4422,7 +4194,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>282</v>
+        <v>224</v>
       </c>
       <c r="B139" t="s">
         <v>141</v>
@@ -4433,7 +4205,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>368</v>
+        <v>228</v>
       </c>
       <c r="B140" t="s">
         <v>141</v>
@@ -4444,159 +4216,153 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
       <c r="B141" t="s">
-        <v>334</v>
-      </c>
-      <c r="C141" t="s">
-        <v>330</v>
+        <v>188</v>
       </c>
       <c r="J141" t="s">
-        <v>329</v>
+        <v>46</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>253</v>
+        <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>254</v>
+        <v>143</v>
       </c>
       <c r="J142" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>256</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>254</v>
+        <v>143</v>
       </c>
       <c r="J143" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>257</v>
+        <v>140</v>
       </c>
       <c r="B144" t="s">
-        <v>254</v>
+        <v>141</v>
       </c>
       <c r="J144" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B145" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="J145" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="B146" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="J146" t="s">
-        <v>255</v>
+        <v>46</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="B147" t="s">
-        <v>328</v>
-      </c>
-      <c r="C147" t="s">
-        <v>330</v>
+        <v>188</v>
       </c>
       <c r="J147" t="s">
-        <v>329</v>
+        <v>46</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>342</v>
       </c>
       <c r="B148" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J148" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>223</v>
+        <v>386</v>
       </c>
       <c r="B149" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J149" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>225</v>
+        <v>346</v>
       </c>
       <c r="B150" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J150" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>227</v>
+        <v>350</v>
       </c>
       <c r="B151" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J151" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>281</v>
+        <v>348</v>
       </c>
       <c r="B152" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J152" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>367</v>
+        <v>336</v>
       </c>
       <c r="B153" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="J153" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
       <c r="B154" t="s">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="J154" t="s">
         <v>46</v>
@@ -4604,10 +4370,10 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>301</v>
+        <v>352</v>
       </c>
       <c r="B155" t="s">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="J155" t="s">
         <v>46</v>
@@ -4615,10 +4381,13 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>44</v>
       </c>
       <c r="B156" t="s">
-        <v>300</v>
+        <v>45</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J156" t="s">
         <v>46</v>
@@ -4626,10 +4395,10 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>304</v>
+        <v>368</v>
       </c>
       <c r="B157" t="s">
-        <v>300</v>
+        <v>141</v>
       </c>
       <c r="J157" t="s">
         <v>46</v>
@@ -4637,7 +4406,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>305</v>
+        <v>369</v>
       </c>
       <c r="B158" t="s">
         <v>300</v>
@@ -4648,21 +4417,21 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>306</v>
+        <v>382</v>
       </c>
       <c r="B159" t="s">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="J159" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>307</v>
+        <v>380</v>
       </c>
       <c r="B160" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="J160" t="s">
         <v>46</v>
@@ -4670,10 +4439,10 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>308</v>
+        <v>381</v>
       </c>
       <c r="B161" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="J161" t="s">
         <v>46</v>
@@ -4681,7 +4450,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>309</v>
+        <v>387</v>
       </c>
       <c r="B162" t="s">
         <v>300</v>
@@ -4692,7 +4461,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>311</v>
+        <v>388</v>
       </c>
       <c r="B163" t="s">
         <v>300</v>
@@ -4703,10 +4472,10 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>312</v>
+        <v>389</v>
       </c>
       <c r="B164" t="s">
-        <v>300</v>
+        <v>137</v>
       </c>
       <c r="J164" t="s">
         <v>46</v>
@@ -4714,195 +4483,426 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="B165" t="s">
-        <v>300</v>
+        <v>141</v>
       </c>
       <c r="J165" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>343</v>
+        <v>261</v>
       </c>
       <c r="B166" t="s">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="J166" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>345</v>
+        <v>270</v>
       </c>
       <c r="B167" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="J167" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>347</v>
+        <v>129</v>
       </c>
       <c r="B168" t="s">
-        <v>300</v>
+        <v>130</v>
+      </c>
+      <c r="E168" t="s">
+        <v>72</v>
+      </c>
+      <c r="F168" t="s">
+        <v>133</v>
+      </c>
+      <c r="G168" t="s">
+        <v>134</v>
+      </c>
+      <c r="H168" t="s">
+        <v>132</v>
+      </c>
+      <c r="I168">
+        <v>0.22</v>
       </c>
       <c r="J168" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>349</v>
+        <v>248</v>
       </c>
       <c r="B169" t="s">
-        <v>300</v>
+        <v>249</v>
+      </c>
+      <c r="E169" t="s">
+        <v>72</v>
+      </c>
+      <c r="F169" t="s">
+        <v>133</v>
+      </c>
+      <c r="G169" t="s">
+        <v>134</v>
+      </c>
+      <c r="H169" t="s">
+        <v>132</v>
+      </c>
+      <c r="I169">
+        <v>0.22</v>
       </c>
       <c r="J169" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>351</v>
+        <v>250</v>
       </c>
       <c r="B170" t="s">
-        <v>300</v>
+        <v>251</v>
+      </c>
+      <c r="E170" t="s">
+        <v>72</v>
+      </c>
+      <c r="F170" t="s">
+        <v>133</v>
+      </c>
+      <c r="G170" t="s">
+        <v>134</v>
+      </c>
+      <c r="H170" t="s">
+        <v>132</v>
+      </c>
+      <c r="I170">
+        <v>0.22</v>
       </c>
       <c r="J170" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>353</v>
+        <v>258</v>
       </c>
       <c r="B171" t="s">
-        <v>300</v>
+        <v>259</v>
+      </c>
+      <c r="E171" t="s">
+        <v>72</v>
+      </c>
+      <c r="F171" t="s">
+        <v>133</v>
+      </c>
+      <c r="G171" t="s">
+        <v>134</v>
+      </c>
+      <c r="H171" t="s">
+        <v>132</v>
+      </c>
+      <c r="I171">
+        <v>0.22</v>
       </c>
       <c r="J171" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>365</v>
+        <v>158</v>
       </c>
       <c r="B172" t="s">
-        <v>300</v>
+        <v>159</v>
+      </c>
+      <c r="E172" t="s">
+        <v>86</v>
+      </c>
+      <c r="F172" t="s">
+        <v>162</v>
+      </c>
+      <c r="G172" t="s">
+        <v>163</v>
+      </c>
+      <c r="H172" t="s">
+        <v>161</v>
+      </c>
+      <c r="I172">
+        <v>7.39</v>
       </c>
       <c r="J172" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>366</v>
+        <v>320</v>
       </c>
       <c r="B173" t="s">
-        <v>300</v>
+        <v>321</v>
+      </c>
+      <c r="E173" t="s">
+        <v>14</v>
+      </c>
+      <c r="F173">
+        <v>1772204</v>
+      </c>
+      <c r="G173" t="s">
+        <v>324</v>
+      </c>
+      <c r="H173" t="s">
+        <v>323</v>
+      </c>
+      <c r="I173">
+        <v>56.5</v>
       </c>
       <c r="J173" t="s">
-        <v>22</v>
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>369</v>
+        <v>229</v>
       </c>
       <c r="B174" t="s">
-        <v>300</v>
+        <v>230</v>
+      </c>
+      <c r="C174" t="s">
+        <v>235</v>
+      </c>
+      <c r="D174" t="s">
+        <v>234</v>
+      </c>
+      <c r="E174" t="s">
+        <v>14</v>
+      </c>
+      <c r="F174">
+        <v>1715855</v>
+      </c>
+      <c r="G174" t="s">
+        <v>233</v>
+      </c>
+      <c r="H174" t="s">
+        <v>232</v>
+      </c>
+      <c r="I174">
+        <v>1.74</v>
       </c>
       <c r="J174" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>370</v>
+        <v>47</v>
       </c>
       <c r="B175" t="s">
-        <v>300</v>
+        <v>48</v>
+      </c>
+      <c r="E175" t="s">
+        <v>14</v>
+      </c>
+      <c r="F175">
+        <v>1696320</v>
+      </c>
+      <c r="G175" t="s">
+        <v>51</v>
+      </c>
+      <c r="H175" t="s">
+        <v>50</v>
+      </c>
+      <c r="I175">
+        <v>4.4000000000000004</v>
       </c>
       <c r="J175" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="B176" t="s">
-        <v>300</v>
+        <v>48</v>
+      </c>
+      <c r="E176" t="s">
+        <v>14</v>
+      </c>
+      <c r="F176">
+        <v>1696320</v>
+      </c>
+      <c r="G176" t="s">
+        <v>51</v>
+      </c>
+      <c r="H176" t="s">
+        <v>50</v>
+      </c>
+      <c r="I176">
+        <v>4.4000000000000004</v>
       </c>
       <c r="J176" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="B177" t="s">
-        <v>300</v>
+        <v>374</v>
+      </c>
+      <c r="D177" t="s">
+        <v>378</v>
+      </c>
+      <c r="E177" t="s">
+        <v>14</v>
+      </c>
+      <c r="F177">
+        <v>1202826</v>
+      </c>
+      <c r="G177" t="s">
+        <v>377</v>
+      </c>
+      <c r="H177" t="s">
+        <v>376</v>
+      </c>
+      <c r="I177">
+        <v>0.29699999999999999</v>
       </c>
       <c r="J177" t="s">
-        <v>46</v>
+        <v>375</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>384</v>
+        <v>82</v>
       </c>
       <c r="B178" t="s">
-        <v>300</v>
+        <v>83</v>
+      </c>
+      <c r="D178" t="s">
+        <v>89</v>
+      </c>
+      <c r="E178" t="s">
+        <v>86</v>
+      </c>
+      <c r="F178" t="s">
+        <v>87</v>
+      </c>
+      <c r="G178" t="s">
+        <v>88</v>
+      </c>
+      <c r="H178" t="s">
+        <v>85</v>
+      </c>
+      <c r="I178">
+        <v>9.58</v>
       </c>
       <c r="J178" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>385</v>
+        <v>26</v>
       </c>
       <c r="B179" t="s">
-        <v>300</v>
+        <v>27</v>
+      </c>
+      <c r="C179" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179" t="s">
+        <v>31</v>
+      </c>
+      <c r="E179" t="s">
+        <v>14</v>
+      </c>
+      <c r="F179">
+        <v>1564957</v>
+      </c>
+      <c r="G179" t="s">
+        <v>30</v>
+      </c>
+      <c r="H179" t="s">
+        <v>29</v>
+      </c>
+      <c r="I179">
+        <v>1.33</v>
       </c>
       <c r="J179" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>387</v>
+        <v>111</v>
       </c>
       <c r="B180" t="s">
-        <v>300</v>
+        <v>112</v>
+      </c>
+      <c r="D180" t="s">
+        <v>116</v>
+      </c>
+      <c r="E180" t="s">
+        <v>14</v>
+      </c>
+      <c r="F180">
+        <v>1084340</v>
+      </c>
+      <c r="G180" t="s">
+        <v>115</v>
+      </c>
+      <c r="H180" t="s">
+        <v>114</v>
+      </c>
+      <c r="I180">
+        <v>0.56499999999999995</v>
       </c>
       <c r="J180" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>388</v>
+        <v>193</v>
       </c>
       <c r="B181" t="s">
-        <v>300</v>
+        <v>194</v>
+      </c>
+      <c r="E181" t="s">
+        <v>14</v>
+      </c>
+      <c r="F181">
+        <v>1842347</v>
+      </c>
+      <c r="G181" t="s">
+        <v>197</v>
+      </c>
+      <c r="H181" t="s">
+        <v>196</v>
+      </c>
+      <c r="I181">
+        <v>0.58099999999999996</v>
       </c>
       <c r="J181" t="s">
-        <v>46</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">
     <sortState ref="A2:J181">
-      <sortCondition ref="F1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>